<commit_message>
adding new project ControlProject
</commit_message>
<xml_diff>
--- a/Python/ControlProject/Kontroller.xlsx
+++ b/Python/ControlProject/Kontroller.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrma\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrma\Desktop\IT-security\Python\ControlProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024E2162-5DE9-4866-9AF9-714267D5C77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664CCD6C-B5F4-4636-8089-AE7D42C5D470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5430" yWindow="6345" windowWidth="22920" windowHeight="8730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>A 7 Human Resources</t>
   </si>
@@ -74,12 +74,6 @@
   </si>
   <si>
     <t>Gmail</t>
-  </si>
-  <si>
-    <t>jensdetermanden</t>
-  </si>
-  <si>
-    <t>kontroldetnu</t>
   </si>
 </sst>
 </file>
@@ -432,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q3:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,9 +507,6 @@
       <c r="P3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -531,9 +522,6 @@
         <v>10</v>
       </c>
       <c r="P4" s="1"/>
-      <c r="Q4" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>